<commit_message>
Update Leaderboard Excel data
</commit_message>
<xml_diff>
--- a/Leaderboard.xlsx
+++ b/Leaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepti\Desktop\Deepti\projectpersonal\leaderboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B266DE27-1AC1-426D-AF82-269AB72E2297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787A8B24-7124-44EC-9A37-566DC0BC85AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{730DF1DB-C3E8-4555-8E91-E2AF207B1844}"/>
   </bookViews>
@@ -694,7 +694,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,7 +762,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Update: new scores in leaderboard
</commit_message>
<xml_diff>
--- a/Leaderboard.xlsx
+++ b/Leaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepti\Desktop\Deepti\projectpersonal\leaderboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CB5E25D-A9E0-4307-BECC-B5033E0208D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD22341-AD6D-4A21-BF73-2FEEA7994F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0E312E4D-B331-491F-9DB8-B3982B9B947D}"/>
   </bookViews>
@@ -474,7 +474,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,7 +520,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Update: Add static images
</commit_message>
<xml_diff>
--- a/Leaderboard.xlsx
+++ b/Leaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepti\Desktop\Deepti\projectpersonal\leaderboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD22341-AD6D-4A21-BF73-2FEEA7994F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1F62E2-0C64-4EBD-8F3D-A468D05FCF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0E312E4D-B331-491F-9DB8-B3982B9B947D}"/>
   </bookViews>
@@ -474,7 +474,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>85</v>
+        <v>785</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>

</xml_diff>